<commit_message>
Update template and optimize reconciliation logic for better performance
</commit_message>
<xml_diff>
--- a/static/sample_template.xlsx
+++ b/static/sample_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Py\GST Reco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Py\GST Reco\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{202D34EF-1383-4B01-9365-B5C2576C50DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B2C5D5-1CD3-4016-9CB3-76D519911967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{44C4A0D1-DDB0-44FF-B53D-7EFFDD78369E}"/>
   </bookViews>
@@ -458,9 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6E29B0-93BA-4B95-8FE0-6B91216FA540}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -484,13 +482,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -526,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>